<commit_message>
CWEs in Excel Datei von Passwörter hinzugefügt
</commit_message>
<xml_diff>
--- a/Anhang/Brute_Force_Plaintext.xlsx
+++ b/Anhang/Brute_Force_Plaintext.xlsx
@@ -5,18 +5,19 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Semester\Unterlagen\Sicherer Programmierung\chess_server_strong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Semester\Unterlagen\Sicherer Programmierung\chess_server_strong\Anhang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A123A2-0060-4C94-A9DE-D22A803FADA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C0F5C1-5281-4534-8CD3-FA76FC7375FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CWSS Score" sheetId="1" r:id="rId1"/>
     <sheet name="Base Finding" sheetId="3" r:id="rId2"/>
     <sheet name="Attack Surface" sheetId="5" r:id="rId3"/>
     <sheet name="Environmental " sheetId="6" r:id="rId4"/>
+    <sheet name="CWE" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="140">
   <si>
     <t xml:space="preserve">The Common Weakness Scoring System (CWSS) provides a mechanism for prioritizing software weaknesses in a consistent, flexible, open manner. </t>
   </si>
@@ -474,6 +475,33 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>Zur Bepunktung herangezogene CWE</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Plaintext Storage of a Password</t>
+  </si>
+  <si>
+    <t>Use of Password System for primary Authentification</t>
+  </si>
+  <si>
+    <t>ClearageStorage of Sensitive Information</t>
+  </si>
+  <si>
+    <t>Weak Password Requirements</t>
+  </si>
+  <si>
+    <t>Insufficiently Protected Credentials</t>
+  </si>
+  <si>
+    <t>Missing Password Field Masking</t>
   </si>
 </sst>
 </file>
@@ -483,7 +511,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,8 +639,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -709,8 +760,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -733,11 +802,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -949,6 +1119,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1274,7 +1501,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -3704,4 +3931,356 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C12E03-251F-4DCA-8481-420E98676B76}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="77"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="80"/>
+    </row>
+    <row r="3" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="84"/>
+    </row>
+    <row r="4" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="81"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
+      <c r="P4" s="87"/>
+    </row>
+    <row r="5" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="88">
+        <v>256</v>
+      </c>
+      <c r="B5" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="90"/>
+    </row>
+    <row r="6" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="88"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="90"/>
+    </row>
+    <row r="7" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="91">
+        <v>309</v>
+      </c>
+      <c r="B7" s="92" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="93"/>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="91"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="92"/>
+      <c r="N8" s="92"/>
+      <c r="O8" s="92"/>
+      <c r="P8" s="93"/>
+    </row>
+    <row r="9" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="88">
+        <v>312</v>
+      </c>
+      <c r="B9" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+      <c r="P9" s="90"/>
+    </row>
+    <row r="10" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="88"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="90"/>
+    </row>
+    <row r="11" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="91">
+        <v>521</v>
+      </c>
+      <c r="B11" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="93"/>
+    </row>
+    <row r="12" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="91"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="92"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="93"/>
+    </row>
+    <row r="13" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="88">
+        <v>522</v>
+      </c>
+      <c r="B13" s="89" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="90"/>
+    </row>
+    <row r="14" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="88"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="90"/>
+    </row>
+    <row r="15" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="91">
+        <v>549</v>
+      </c>
+      <c r="B15" s="92" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="92"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="93"/>
+    </row>
+    <row r="16" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="91"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="92"/>
+      <c r="O16" s="92"/>
+      <c r="P16" s="93"/>
+    </row>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:P16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:P10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:P12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:P14"/>
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:P4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:P6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:P8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>